<commit_message>
data drivern framework with excel
</commit_message>
<xml_diff>
--- a/src/test/resources/registration.xlsx
+++ b/src/test/resources/registration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>MMM</t>
-  </si>
-  <si>
     <t>fm@kmail.com</t>
   </si>
   <si>
@@ -87,17 +84,38 @@
     <t>Faiza</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>faruq</t>
+  </si>
+  <si>
+    <t>faruq@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking </t>
+  </si>
+  <si>
+    <t>saving</t>
+  </si>
+  <si>
+    <t>Molla</t>
+  </si>
+  <si>
+    <t>Fima</t>
+  </si>
+  <si>
+    <t>Nisa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +130,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,16 +156,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,12 +475,14 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -481,81 +514,84 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
+      <c r="I2">
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -569,24 +605,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix chorme open issue adding bonnie garcia dependency
</commit_message>
<xml_diff>
--- a/src/test/resources/registration.xlsx
+++ b/src/test/resources/registration.xlsx
@@ -475,7 +475,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -536,9 +536,6 @@
       </c>
       <c r="H2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="I2">
-        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:9">

</xml_diff>